<commit_message>
begin creation revised and updated full dataset
</commit_message>
<xml_diff>
--- a/pop_meta.xlsx
+++ b/pop_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/ST-IPM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="11_501C1CC78F79A8D366075C52F37BD2724A4446D1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E0A8A9E-DEFF-433A-BF03-7682D6C45D5E}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="11_501C1CC78F79A8D366075C52F37BD2724A4446D1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CCAB8671-DE4D-406F-BEA9-D1E6139DA95E}"/>
   <bookViews>
     <workbookView xWindow="-12740" yWindow="-20060" windowWidth="28410" windowHeight="15550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,12 +160,6 @@
     <t>Willapa Bay Natural</t>
   </si>
   <si>
-    <t>FRAM_StockID</t>
-  </si>
-  <si>
-    <t>FRAM_StockLongName</t>
-  </si>
-  <si>
     <t>Area 10 Miscellaneous Wild UnMarked</t>
   </si>
   <si>
@@ -395,6 +389,12 @@
   </si>
   <si>
     <t>hab_km</t>
+  </si>
+  <si>
+    <t>StockID</t>
+  </si>
+  <si>
+    <t>StockLongName</t>
   </si>
 </sst>
 </file>
@@ -819,24 +819,24 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="8" width="10" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" customWidth="1"/>
-    <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="9" max="10" width="10" customWidth="1"/>
+    <col min="11" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" customWidth="1"/>
     <col min="17" max="17" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -848,52 +848,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -904,43 +904,43 @@
         <v>9</v>
       </c>
       <c r="C2">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2">
         <v>-122.465661</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>47.668698999999997</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>39.9</v>
       </c>
-      <c r="H2">
-        <v>1986</v>
-      </c>
-      <c r="I2">
+      <c r="J2">
+        <v>1986</v>
+      </c>
+      <c r="K2">
         <v>2017</v>
       </c>
-      <c r="J2">
-        <v>32</v>
-      </c>
-      <c r="K2">
-        <v>32</v>
-      </c>
       <c r="L2">
         <v>32</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O2">
-        <v>105</v>
-      </c>
-      <c r="P2" t="s">
-        <v>47</v>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -951,43 +951,43 @@
         <v>10</v>
       </c>
       <c r="C3">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3">
         <v>-122.8242</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>47.589599999999997</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>130.80000000000001</v>
       </c>
-      <c r="H3">
-        <v>1986</v>
-      </c>
-      <c r="I3">
+      <c r="J3">
+        <v>1986</v>
+      </c>
+      <c r="K3">
         <v>2017</v>
       </c>
-      <c r="J3">
-        <v>32</v>
-      </c>
-      <c r="K3">
-        <v>32</v>
-      </c>
       <c r="L3">
         <v>32</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O3">
-        <v>93</v>
-      </c>
-      <c r="P3" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -998,46 +998,46 @@
         <v>11</v>
       </c>
       <c r="C4">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4">
         <v>-122.45249200000001</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>47.388660999999999</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>44.8</v>
       </c>
-      <c r="H4">
-        <v>1986</v>
-      </c>
-      <c r="I4">
+      <c r="J4">
+        <v>1986</v>
+      </c>
+      <c r="K4">
         <v>2017</v>
       </c>
-      <c r="J4">
-        <v>32</v>
-      </c>
-      <c r="K4">
-        <v>32</v>
-      </c>
       <c r="L4">
         <v>32</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O4">
-        <v>89</v>
-      </c>
-      <c r="P4" t="s">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1048,49 +1048,49 @@
         <v>12</v>
       </c>
       <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5">
         <v>-122.7836076</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>47.651915930000001</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>95.4</v>
       </c>
-      <c r="F5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1986</v>
+      <c r="H5" t="s">
+        <v>102</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1986</v>
+      </c>
+      <c r="K5">
         <v>2017</v>
       </c>
-      <c r="J5">
-        <v>32</v>
-      </c>
-      <c r="K5">
-        <v>32</v>
-      </c>
       <c r="L5">
         <v>32</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N5">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>30</v>
       </c>
-      <c r="O5">
-        <v>45</v>
-      </c>
-      <c r="P5" t="s">
-        <v>50</v>
-      </c>
       <c r="Q5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1101,49 +1101,49 @@
         <v>13</v>
       </c>
       <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6">
         <v>-122.859826</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>47.825445000000002</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>76.3</v>
       </c>
-      <c r="F6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6">
+      <c r="H6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="H6">
-        <v>1986</v>
-      </c>
-      <c r="I6">
+      <c r="J6">
+        <v>1986</v>
+      </c>
+      <c r="K6">
         <v>2017</v>
       </c>
-      <c r="J6">
-        <v>32</v>
-      </c>
-      <c r="K6">
-        <v>32</v>
-      </c>
       <c r="L6">
         <v>32</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N6">
+        <v>32</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>25</v>
       </c>
-      <c r="O6">
-        <v>51</v>
-      </c>
-      <c r="P6" t="s">
-        <v>51</v>
-      </c>
       <c r="Q6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1154,43 +1154,43 @@
         <v>14</v>
       </c>
       <c r="C7">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7">
         <v>-123.119288</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>47.364944000000001</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>202.7</v>
       </c>
-      <c r="H7">
-        <v>1986</v>
-      </c>
-      <c r="I7">
+      <c r="J7">
+        <v>1986</v>
+      </c>
+      <c r="K7">
         <v>2017</v>
       </c>
-      <c r="J7">
-        <v>32</v>
-      </c>
-      <c r="K7">
-        <v>32</v>
-      </c>
       <c r="L7">
         <v>32</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O7">
-        <v>55</v>
-      </c>
-      <c r="P7" t="s">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1201,49 +1201,49 @@
         <v>15</v>
       </c>
       <c r="C8">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8">
         <v>-123.01589439999999</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>47.262432660000002</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>64.8</v>
       </c>
-      <c r="F8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>1986</v>
+      <c r="H8" t="s">
+        <v>106</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1986</v>
+      </c>
+      <c r="K8">
         <v>2017</v>
       </c>
-      <c r="J8">
-        <v>32</v>
-      </c>
-      <c r="K8">
-        <v>32</v>
-      </c>
       <c r="L8">
         <v>32</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N8">
+        <v>32</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>5</v>
       </c>
-      <c r="O8">
-        <v>75</v>
-      </c>
-      <c r="P8" t="s">
-        <v>53</v>
-      </c>
       <c r="Q8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1254,43 +1254,43 @@
         <v>16</v>
       </c>
       <c r="C9">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9">
         <v>-122.702698</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>47.264969000000001</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>46.7</v>
       </c>
-      <c r="H9">
-        <v>1986</v>
-      </c>
-      <c r="I9">
+      <c r="J9">
+        <v>1986</v>
+      </c>
+      <c r="K9">
         <v>2017</v>
-      </c>
-      <c r="J9">
-        <v>31</v>
-      </c>
-      <c r="K9">
-        <v>31</v>
       </c>
       <c r="L9">
         <v>31</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O9">
-        <v>81</v>
-      </c>
-      <c r="P9" t="s">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1301,43 +1301,43 @@
         <v>17</v>
       </c>
       <c r="C10">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10">
         <v>-122.82063599999999</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>47.195821000000002</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>360.9</v>
       </c>
-      <c r="H10">
-        <v>1986</v>
-      </c>
-      <c r="I10">
+      <c r="J10">
+        <v>1986</v>
+      </c>
+      <c r="K10">
         <v>2017</v>
       </c>
-      <c r="J10">
-        <v>32</v>
-      </c>
-      <c r="K10">
-        <v>32</v>
-      </c>
       <c r="L10">
         <v>32</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O10">
-        <v>61</v>
-      </c>
-      <c r="P10" t="s">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1348,46 +1348,46 @@
         <v>18</v>
       </c>
       <c r="C11" s="3">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="3">
         <v>-122.733811</v>
       </c>
-      <c r="D11" s="3">
+      <c r="F11" s="3">
         <v>48.972937000000002</v>
       </c>
-      <c r="E11" s="3">
+      <c r="G11" s="3">
         <v>115.1</v>
       </c>
-      <c r="H11" s="3">
-        <v>1986</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
+        <v>1986</v>
+      </c>
+      <c r="K11" s="3">
         <v>2017</v>
       </c>
-      <c r="J11" s="3">
-        <v>32</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
+        <v>32</v>
+      </c>
+      <c r="M11" s="3">
         <v>31</v>
       </c>
-      <c r="L11" s="3">
+      <c r="N11" s="3">
         <v>31</v>
       </c>
-      <c r="M11" s="3">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
       <c r="O11" s="3">
-        <v>13</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>56</v>
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1398,49 +1398,49 @@
         <v>19</v>
       </c>
       <c r="C12">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12">
         <v>-122.47416200000001</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>48.359836999999999</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>102.1</v>
       </c>
-      <c r="F12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>1986</v>
+      <c r="H12" t="s">
+        <v>107</v>
       </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1986</v>
+      </c>
+      <c r="K12">
         <v>2017</v>
       </c>
-      <c r="J12">
-        <v>32</v>
-      </c>
-      <c r="K12">
-        <v>32</v>
-      </c>
       <c r="L12">
         <v>32</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N12">
+        <v>32</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>22</v>
       </c>
-      <c r="O12">
-        <v>23</v>
-      </c>
-      <c r="P12" t="s">
-        <v>98</v>
-      </c>
       <c r="Q12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1451,52 +1451,52 @@
         <v>20</v>
       </c>
       <c r="C13" s="6">
+        <v>149</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="6">
         <v>-124.1692596</v>
       </c>
-      <c r="D13" s="6">
+      <c r="F13" s="6">
         <v>46.91656476</v>
       </c>
-      <c r="E13" s="6">
+      <c r="G13" s="6">
         <v>2514.1999999999998</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1986</v>
+      <c r="H13" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1986</v>
+      </c>
+      <c r="K13" s="6">
         <v>2018</v>
       </c>
-      <c r="J13" s="6">
+      <c r="L13" s="6">
         <v>33</v>
       </c>
-      <c r="K13" s="6">
-        <v>32</v>
-      </c>
-      <c r="L13" s="6">
-        <v>32</v>
-      </c>
       <c r="M13" s="6">
         <v>32</v>
       </c>
       <c r="N13" s="6">
+        <v>32</v>
+      </c>
+      <c r="O13" s="6">
+        <v>32</v>
+      </c>
+      <c r="P13" s="6">
         <v>30</v>
       </c>
-      <c r="O13" s="6">
-        <v>149</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="Q13" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1507,49 +1507,49 @@
         <v>21</v>
       </c>
       <c r="C14">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14">
         <v>-122.9091057</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>47.043614419999997</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>132.30000000000001</v>
       </c>
-      <c r="F14" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>1986</v>
+      <c r="H14" t="s">
+        <v>109</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>1986</v>
+      </c>
+      <c r="K14">
         <v>2018</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>33</v>
       </c>
-      <c r="K14">
-        <v>32</v>
-      </c>
-      <c r="L14">
-        <v>32</v>
-      </c>
       <c r="M14">
+        <v>32</v>
+      </c>
+      <c r="N14">
+        <v>32</v>
+      </c>
+      <c r="O14">
         <v>33</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>18</v>
       </c>
-      <c r="O14">
-        <v>63</v>
-      </c>
-      <c r="P14" t="s">
-        <v>95</v>
-      </c>
       <c r="Q14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1560,52 +1560,52 @@
         <v>22</v>
       </c>
       <c r="C15" s="4">
+        <v>107</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="4">
         <v>-123.129772</v>
       </c>
-      <c r="D15" s="4">
+      <c r="F15" s="4">
         <v>48.152718</v>
       </c>
-      <c r="E15" s="4">
+      <c r="G15" s="4">
         <v>129.69999999999999</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="4">
         <v>1</v>
       </c>
-      <c r="H15" s="4">
-        <v>1986</v>
-      </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
+        <v>1986</v>
+      </c>
+      <c r="K15" s="4">
         <v>2017</v>
       </c>
-      <c r="J15" s="4">
-        <v>32</v>
-      </c>
-      <c r="K15" s="4">
-        <v>32</v>
-      </c>
       <c r="L15" s="4">
         <v>32</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="4">
+        <v>32</v>
+      </c>
+      <c r="N15" s="4">
+        <v>32</v>
+      </c>
+      <c r="O15" s="2">
         <v>13</v>
       </c>
-      <c r="N15" s="4">
+      <c r="P15" s="4">
         <v>10</v>
       </c>
-      <c r="O15" s="4">
-        <v>107</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="Q15" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1616,43 +1616,43 @@
         <v>23</v>
       </c>
       <c r="C16">
+        <v>115</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16">
         <v>-123.0051816</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>48.023348120000001</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>301.3</v>
       </c>
-      <c r="H16">
-        <v>1986</v>
-      </c>
-      <c r="I16">
+      <c r="J16">
+        <v>1986</v>
+      </c>
+      <c r="K16">
         <v>2017</v>
       </c>
-      <c r="J16">
-        <v>32</v>
-      </c>
-      <c r="K16">
-        <v>32</v>
-      </c>
       <c r="L16">
         <v>32</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O16">
-        <v>115</v>
-      </c>
-      <c r="P16" t="s">
-        <v>92</v>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
       </c>
       <c r="Q16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1663,46 +1663,46 @@
         <v>24</v>
       </c>
       <c r="C17" s="5">
+        <v>111</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="5">
         <v>-123.56963399999999</v>
       </c>
-      <c r="D17" s="5">
+      <c r="F17" s="5">
         <v>48.148155000000003</v>
       </c>
-      <c r="E17" s="5">
+      <c r="G17" s="5">
         <v>13.7</v>
       </c>
-      <c r="H17" s="5">
-        <v>1986</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="J17" s="5">
+        <v>1986</v>
+      </c>
+      <c r="K17" s="5">
         <v>2017</v>
       </c>
-      <c r="J17" s="5">
-        <v>32</v>
-      </c>
-      <c r="K17" s="5">
-        <v>32</v>
-      </c>
       <c r="L17" s="5">
         <v>32</v>
       </c>
       <c r="M17" s="5">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N17" s="5">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O17" s="5">
-        <v>111</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1713,46 +1713,46 @@
         <v>25</v>
       </c>
       <c r="C18" s="6">
+        <v>157</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="6">
         <v>-124.03316599999999</v>
       </c>
-      <c r="D18" s="6">
+      <c r="F18" s="6">
         <v>46.939467</v>
       </c>
-      <c r="E18" s="6">
+      <c r="G18" s="6">
         <v>211</v>
       </c>
-      <c r="H18" s="6">
-        <v>1986</v>
-      </c>
-      <c r="I18" s="6">
+      <c r="J18" s="6">
+        <v>1986</v>
+      </c>
+      <c r="K18" s="6">
         <v>2017</v>
       </c>
-      <c r="J18" s="6">
-        <v>32</v>
-      </c>
-      <c r="K18" s="6">
+      <c r="L18" s="6">
+        <v>32</v>
+      </c>
+      <c r="M18" s="6">
         <v>30</v>
       </c>
-      <c r="L18" s="6">
+      <c r="N18" s="6">
         <v>30</v>
       </c>
-      <c r="M18" s="6">
-        <v>0</v>
-      </c>
-      <c r="N18" s="6">
-        <v>0</v>
-      </c>
       <c r="O18" s="6">
-        <v>157</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1763,52 +1763,52 @@
         <v>26</v>
       </c>
       <c r="C19" s="4">
+        <v>97</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="4">
         <v>-122.2145</v>
       </c>
-      <c r="D19" s="4">
+      <c r="F19" s="4">
         <v>47.351900000000001</v>
       </c>
-      <c r="E19" s="4">
+      <c r="G19" s="4">
         <v>339.3</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="4">
         <v>1</v>
       </c>
-      <c r="H19" s="4">
-        <v>1986</v>
-      </c>
-      <c r="I19" s="4">
+      <c r="J19" s="4">
+        <v>1986</v>
+      </c>
+      <c r="K19" s="4">
         <v>2018</v>
       </c>
-      <c r="J19" s="4">
+      <c r="L19" s="4">
         <v>33</v>
       </c>
-      <c r="K19" s="4">
-        <v>32</v>
-      </c>
-      <c r="L19" s="4">
-        <v>32</v>
-      </c>
-      <c r="M19" s="2">
+      <c r="M19" s="4">
+        <v>32</v>
+      </c>
+      <c r="N19" s="4">
+        <v>32</v>
+      </c>
+      <c r="O19" s="2">
         <v>19</v>
       </c>
-      <c r="N19" s="4">
+      <c r="P19" s="4">
         <v>28</v>
       </c>
-      <c r="O19" s="4">
-        <v>97</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="Q19" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -1819,43 +1819,43 @@
         <v>27</v>
       </c>
       <c r="C20">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20">
         <v>-124.43052</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>47.749116000000001</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>263.10000000000002</v>
       </c>
-      <c r="H20">
-        <v>1986</v>
-      </c>
-      <c r="I20">
+      <c r="J20">
+        <v>1986</v>
+      </c>
+      <c r="K20">
         <v>2017</v>
       </c>
-      <c r="J20">
-        <v>32</v>
-      </c>
-      <c r="K20">
-        <v>32</v>
-      </c>
       <c r="L20">
         <v>32</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O20">
-        <v>135</v>
-      </c>
-      <c r="P20" t="s">
-        <v>84</v>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
       </c>
       <c r="Q20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1866,43 +1866,43 @@
         <v>28</v>
       </c>
       <c r="C21" s="6">
+        <v>153</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="6">
         <v>-124.054237</v>
       </c>
-      <c r="D21" s="6">
+      <c r="F21" s="6">
         <v>47.040880999999999</v>
       </c>
-      <c r="E21" s="6">
+      <c r="G21" s="6">
         <v>268.60000000000002</v>
       </c>
-      <c r="H21" s="6">
-        <v>1986</v>
-      </c>
-      <c r="I21" s="6">
+      <c r="J21" s="6">
+        <v>1986</v>
+      </c>
+      <c r="K21" s="6">
         <v>2017</v>
       </c>
-      <c r="J21" s="6">
-        <v>32</v>
-      </c>
-      <c r="K21" s="6">
-        <v>32</v>
-      </c>
       <c r="L21" s="6">
         <v>32</v>
       </c>
       <c r="M21" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N21" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O21" s="6">
-        <v>153</v>
-      </c>
-      <c r="P21" s="6" t="s">
-        <v>82</v>
+        <v>0</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1913,46 +1913,46 @@
         <v>29</v>
       </c>
       <c r="C22" s="4">
+        <v>101</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="4">
         <v>-122.26042940000001</v>
       </c>
-      <c r="D22" s="4">
+      <c r="F22" s="4">
         <v>47.644992790000003</v>
       </c>
-      <c r="E22" s="4">
+      <c r="G22" s="4">
         <v>513.29999999999995</v>
       </c>
-      <c r="H22" s="4">
-        <v>1986</v>
-      </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
+        <v>1986</v>
+      </c>
+      <c r="K22" s="4">
         <v>2017</v>
       </c>
-      <c r="J22" s="4">
-        <v>32</v>
-      </c>
-      <c r="K22" s="4">
-        <v>32</v>
-      </c>
       <c r="L22" s="4">
         <v>32</v>
       </c>
       <c r="M22" s="4">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N22" s="4">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O22" s="4">
-        <v>101</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>78</v>
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -1963,49 +1963,49 @@
         <v>30</v>
       </c>
       <c r="C23">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23">
         <v>-122.70121159999999</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>47.088108669999997</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>317.60000000000002</v>
       </c>
-      <c r="F23" t="s">
-        <v>114</v>
-      </c>
-      <c r="G23">
+      <c r="H23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23">
         <v>1</v>
       </c>
-      <c r="H23">
-        <v>1986</v>
-      </c>
-      <c r="I23">
+      <c r="J23">
+        <v>1986</v>
+      </c>
+      <c r="K23">
         <v>2018</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>33</v>
       </c>
-      <c r="K23">
-        <v>32</v>
-      </c>
-      <c r="L23">
-        <v>32</v>
-      </c>
       <c r="M23">
+        <v>32</v>
+      </c>
+      <c r="N23">
+        <v>32</v>
+      </c>
+      <c r="O23">
         <v>10</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>23</v>
       </c>
-      <c r="O23">
-        <v>69</v>
-      </c>
-      <c r="P23" t="s">
-        <v>77</v>
-      </c>
       <c r="Q23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2016,52 +2016,52 @@
         <v>31</v>
       </c>
       <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="5">
         <v>-122.597909</v>
       </c>
-      <c r="D24" s="5">
+      <c r="F24" s="5">
         <v>48.776489120000001</v>
       </c>
-      <c r="E24" s="5">
+      <c r="G24" s="5">
         <v>692.5</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="H24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="5">
         <v>1</v>
       </c>
-      <c r="H24" s="5">
-        <v>1986</v>
-      </c>
-      <c r="I24" s="5">
+      <c r="J24" s="5">
+        <v>1986</v>
+      </c>
+      <c r="K24" s="5">
         <v>2018</v>
       </c>
-      <c r="J24" s="5">
+      <c r="L24" s="5">
         <v>33</v>
       </c>
-      <c r="K24" s="5">
-        <v>32</v>
-      </c>
-      <c r="L24" s="5">
-        <v>32</v>
-      </c>
-      <c r="M24" s="2">
+      <c r="M24" s="5">
+        <v>32</v>
+      </c>
+      <c r="N24" s="5">
+        <v>32</v>
+      </c>
+      <c r="O24" s="2">
         <v>14</v>
       </c>
-      <c r="N24" s="5">
+      <c r="P24" s="5">
         <v>29</v>
       </c>
-      <c r="O24" s="5">
-        <v>1</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="Q24" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2072,46 +2072,46 @@
         <v>32</v>
       </c>
       <c r="C25" s="3">
+        <v>43</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="3">
         <v>-122.57560700000001</v>
       </c>
-      <c r="D25" s="3">
+      <c r="F25" s="3">
         <v>47.833956000000001</v>
       </c>
-      <c r="E25" s="3">
+      <c r="G25" s="3">
         <v>12.8</v>
       </c>
-      <c r="H25" s="3">
-        <v>1986</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
+        <v>1986</v>
+      </c>
+      <c r="K25" s="3">
         <v>2017</v>
       </c>
-      <c r="J25" s="3">
+      <c r="L25" s="3">
         <v>26</v>
       </c>
-      <c r="K25" s="3">
+      <c r="M25" s="3">
         <v>25</v>
       </c>
-      <c r="L25" s="3">
+      <c r="N25" s="3">
         <v>25</v>
       </c>
-      <c r="M25" s="3">
-        <v>0</v>
-      </c>
-      <c r="N25" s="3">
-        <v>0</v>
-      </c>
       <c r="O25" s="3">
-        <v>43</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>75</v>
+        <v>0</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -2122,49 +2122,49 @@
         <v>33</v>
       </c>
       <c r="C26">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26">
         <v>-122.4268386</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>47.268497920000001</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>580.1</v>
       </c>
-      <c r="F26" t="s">
-        <v>116</v>
-      </c>
-      <c r="G26">
+      <c r="H26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26">
         <v>1</v>
       </c>
-      <c r="H26">
-        <v>1986</v>
-      </c>
-      <c r="I26">
+      <c r="J26">
+        <v>1986</v>
+      </c>
+      <c r="K26">
         <v>2018</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>33</v>
       </c>
-      <c r="K26">
-        <v>32</v>
-      </c>
-      <c r="L26">
-        <v>32</v>
-      </c>
       <c r="M26">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N26">
+        <v>32</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
         <v>30</v>
       </c>
-      <c r="O26">
-        <v>85</v>
-      </c>
-      <c r="P26" t="s">
-        <v>74</v>
-      </c>
       <c r="Q26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2175,43 +2175,43 @@
         <v>34</v>
       </c>
       <c r="C27" s="6">
+        <v>139</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="6">
         <v>-124.3542841</v>
       </c>
-      <c r="D27" s="6">
+      <c r="F27" s="6">
         <v>47.53794224</v>
       </c>
-      <c r="E27" s="6">
+      <c r="G27" s="6">
         <v>381.2</v>
       </c>
-      <c r="H27" s="6">
-        <v>1986</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="J27" s="6">
+        <v>1986</v>
+      </c>
+      <c r="K27" s="6">
         <v>2018</v>
       </c>
-      <c r="J27" s="6">
+      <c r="L27" s="6">
         <v>33</v>
       </c>
-      <c r="K27" s="6">
-        <v>32</v>
-      </c>
-      <c r="L27" s="6">
-        <v>32</v>
-      </c>
       <c r="M27" s="6">
+        <v>32</v>
+      </c>
+      <c r="N27" s="6">
+        <v>32</v>
+      </c>
+      <c r="O27" s="6">
         <v>33</v>
       </c>
-      <c r="N27" s="6">
-        <v>0</v>
-      </c>
-      <c r="O27" s="6">
-        <v>139</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>72</v>
+      <c r="P27" s="6">
+        <v>0</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -2222,43 +2222,43 @@
         <v>35</v>
       </c>
       <c r="C28">
+        <v>131</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28">
         <v>-124.64317</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>47.907395000000001</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>761.6</v>
       </c>
-      <c r="H28">
-        <v>1986</v>
-      </c>
-      <c r="I28">
+      <c r="J28">
+        <v>1986</v>
+      </c>
+      <c r="K28">
         <v>2017</v>
       </c>
-      <c r="J28">
-        <v>32</v>
-      </c>
-      <c r="K28">
-        <v>32</v>
-      </c>
       <c r="L28">
+        <v>32</v>
+      </c>
+      <c r="M28">
+        <v>32</v>
+      </c>
+      <c r="N28">
         <v>30</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
       <c r="O28">
-        <v>131</v>
-      </c>
-      <c r="P28" t="s">
-        <v>71</v>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
       </c>
       <c r="Q28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -2269,43 +2269,43 @@
         <v>36</v>
       </c>
       <c r="C29">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29">
         <v>-124.64317</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>47.907395000000001</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>19.3</v>
       </c>
-      <c r="H29">
-        <v>1986</v>
-      </c>
-      <c r="I29">
+      <c r="J29">
+        <v>1986</v>
+      </c>
+      <c r="K29">
         <v>2017</v>
       </c>
-      <c r="J29">
-        <v>32</v>
-      </c>
-      <c r="K29">
-        <v>32</v>
-      </c>
       <c r="L29">
+        <v>32</v>
+      </c>
+      <c r="M29">
+        <v>32</v>
+      </c>
+      <c r="N29">
         <v>30</v>
       </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
       <c r="O29">
-        <v>127</v>
-      </c>
-      <c r="P29" t="s">
-        <v>70</v>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
       </c>
       <c r="Q29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2316,52 +2316,52 @@
         <v>37</v>
       </c>
       <c r="C30" s="6">
+        <v>145</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="6">
         <v>-124.29792399999999</v>
       </c>
-      <c r="D30" s="6">
+      <c r="F30" s="6">
         <v>47.348188999999998</v>
       </c>
-      <c r="E30" s="6">
+      <c r="G30" s="6">
         <v>234.3</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G30" s="6">
+      <c r="H30" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I30" s="6">
         <v>1</v>
       </c>
-      <c r="H30" s="6">
-        <v>1986</v>
-      </c>
-      <c r="I30" s="6">
+      <c r="J30" s="6">
+        <v>1986</v>
+      </c>
+      <c r="K30" s="6">
         <v>2017</v>
       </c>
-      <c r="J30" s="6">
-        <v>32</v>
-      </c>
-      <c r="K30" s="6">
-        <v>32</v>
-      </c>
       <c r="L30" s="6">
         <v>32</v>
       </c>
       <c r="M30" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N30" s="6">
+        <v>32</v>
+      </c>
+      <c r="O30" s="6">
+        <v>0</v>
+      </c>
+      <c r="P30" s="6">
         <v>29</v>
       </c>
-      <c r="O30" s="6">
-        <v>145</v>
-      </c>
-      <c r="P30" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="Q30" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2372,43 +2372,43 @@
         <v>38</v>
       </c>
       <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31">
         <v>-122.45678270000001</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>48.554918190000002</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>188.2</v>
       </c>
-      <c r="H31">
-        <v>1986</v>
-      </c>
-      <c r="I31">
+      <c r="J31">
+        <v>1986</v>
+      </c>
+      <c r="K31">
         <v>2018</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>33</v>
       </c>
-      <c r="K31">
-        <v>32</v>
-      </c>
-      <c r="L31">
-        <v>32</v>
-      </c>
       <c r="M31">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O31">
-        <v>11</v>
-      </c>
-      <c r="P31" t="s">
-        <v>67</v>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
       </c>
       <c r="Q31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -2419,49 +2419,49 @@
         <v>39</v>
       </c>
       <c r="C32">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32">
         <v>-122.3665</v>
       </c>
-      <c r="D32">
+      <c r="F32">
         <v>48.388056259999999</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>1050.5999999999999</v>
       </c>
-      <c r="F32" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32">
+      <c r="H32" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32">
         <v>1</v>
       </c>
-      <c r="H32">
-        <v>1986</v>
-      </c>
-      <c r="I32">
+      <c r="J32">
+        <v>1986</v>
+      </c>
+      <c r="K32">
         <v>2018</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>33</v>
       </c>
-      <c r="K32">
-        <v>32</v>
-      </c>
-      <c r="L32">
-        <v>32</v>
-      </c>
       <c r="M32">
+        <v>32</v>
+      </c>
+      <c r="N32">
+        <v>32</v>
+      </c>
+      <c r="O32">
         <v>29</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>21</v>
       </c>
-      <c r="O32">
-        <v>17</v>
-      </c>
-      <c r="P32" t="s">
-        <v>65</v>
-      </c>
       <c r="Q32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -2472,49 +2472,49 @@
         <v>40</v>
       </c>
       <c r="C33">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33">
         <v>-123.11765699999999</v>
       </c>
-      <c r="D33">
+      <c r="F33">
         <v>47.339776000000001</v>
       </c>
-      <c r="E33">
+      <c r="G33">
         <v>106.1</v>
       </c>
-      <c r="F33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33">
+      <c r="H33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I33">
         <v>1</v>
       </c>
-      <c r="H33">
-        <v>1986</v>
-      </c>
-      <c r="I33">
+      <c r="J33">
+        <v>1986</v>
+      </c>
+      <c r="K33">
         <v>2017</v>
       </c>
-      <c r="J33">
-        <v>32</v>
-      </c>
-      <c r="K33">
-        <v>32</v>
-      </c>
       <c r="L33">
         <v>32</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N33">
+        <v>32</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
         <v>29</v>
       </c>
-      <c r="O33">
+      <c r="Q33" t="s">
         <v>59</v>
-      </c>
-      <c r="P33" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -2525,43 +2525,43 @@
         <v>41</v>
       </c>
       <c r="C34">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34">
         <v>-122.19891389999999</v>
       </c>
-      <c r="D34">
+      <c r="F34">
         <v>48.020066790000001</v>
       </c>
-      <c r="E34">
+      <c r="G34">
         <v>1358.8</v>
       </c>
-      <c r="H34">
-        <v>1986</v>
-      </c>
-      <c r="I34">
+      <c r="J34">
+        <v>1986</v>
+      </c>
+      <c r="K34">
         <v>2018</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>33</v>
       </c>
-      <c r="K34">
-        <v>32</v>
-      </c>
-      <c r="L34">
-        <v>32</v>
-      </c>
       <c r="M34">
+        <v>32</v>
+      </c>
+      <c r="N34">
+        <v>32</v>
+      </c>
+      <c r="O34">
         <v>15</v>
       </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <v>35</v>
-      </c>
-      <c r="P34" t="s">
-        <v>63</v>
+      <c r="P34">
+        <v>0</v>
       </c>
       <c r="Q34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -2572,43 +2572,43 @@
         <v>42</v>
       </c>
       <c r="C35">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35">
         <v>-122.39026749999999</v>
       </c>
-      <c r="D35">
+      <c r="F35">
         <v>48.243896329999998</v>
       </c>
-      <c r="E35">
+      <c r="G35">
         <v>694.2</v>
       </c>
-      <c r="H35">
-        <v>1986</v>
-      </c>
-      <c r="I35">
+      <c r="J35">
+        <v>1986</v>
+      </c>
+      <c r="K35">
         <v>2018</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>33</v>
       </c>
-      <c r="K35">
-        <v>32</v>
-      </c>
-      <c r="L35">
-        <v>32</v>
-      </c>
       <c r="M35">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O35">
-        <v>29</v>
-      </c>
-      <c r="P35" t="s">
-        <v>62</v>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
       </c>
       <c r="Q35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -2619,43 +2619,43 @@
         <v>43</v>
       </c>
       <c r="C36">
+        <v>117</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36">
         <v>-123.7042368</v>
       </c>
-      <c r="D36">
+      <c r="F36">
         <v>48.155695020000003</v>
       </c>
-      <c r="E36">
+      <c r="G36">
         <v>242.2</v>
       </c>
-      <c r="H36">
-        <v>1986</v>
-      </c>
-      <c r="I36">
+      <c r="J36">
+        <v>1986</v>
+      </c>
+      <c r="K36">
         <v>2017</v>
       </c>
-      <c r="J36">
-        <v>32</v>
-      </c>
-      <c r="K36">
-        <v>32</v>
-      </c>
       <c r="L36">
         <v>32</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O36">
-        <v>117</v>
-      </c>
-      <c r="P36" t="s">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
       </c>
       <c r="Q36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -2666,49 +2666,49 @@
         <v>44</v>
       </c>
       <c r="C37">
+        <v>161</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37">
         <v>-124.09049</v>
       </c>
-      <c r="D37">
+      <c r="F37">
         <v>46.723579000000001</v>
       </c>
-      <c r="E37">
+      <c r="G37">
         <v>2028.2</v>
       </c>
-      <c r="F37" t="s">
-        <v>120</v>
-      </c>
-      <c r="G37">
+      <c r="H37" t="s">
+        <v>118</v>
+      </c>
+      <c r="I37">
         <v>1</v>
       </c>
-      <c r="H37">
-        <v>1986</v>
-      </c>
-      <c r="I37">
+      <c r="J37">
+        <v>1986</v>
+      </c>
+      <c r="K37">
         <v>2017</v>
       </c>
-      <c r="J37">
-        <v>32</v>
-      </c>
-      <c r="K37">
-        <v>32</v>
-      </c>
       <c r="L37">
         <v>32</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N37">
+        <v>32</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
         <v>23</v>
       </c>
-      <c r="O37">
-        <v>161</v>
-      </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>57</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added smolt data updates, revised around single fulljoin dataset ingest
</commit_message>
<xml_diff>
--- a/pop_meta.xlsx
+++ b/pop_meta.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/ST-IPM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="11_501C1CC78F79A8D366075C52F37BD2724A4446D1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CCAB8671-DE4D-406F-BEA9-D1E6139DA95E}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="11_501C1CC78F79A8D366075C52F37BD2724A4446D1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A5DE11C9-E15D-4567-AC1E-25C74DE838F3}"/>
   <bookViews>
-    <workbookView xWindow="-12740" yWindow="-20060" windowWidth="28410" windowHeight="15550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10150" yWindow="-14890" windowWidth="22450" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$35</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
   <si>
     <t>pop_id</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Area 13B Miscellaneous Wild</t>
   </si>
   <si>
-    <t>Area 7-7A Independent Wild</t>
-  </si>
-  <si>
     <t>Baker (Skagit) Wild</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Nooksack River Wild</t>
   </si>
   <si>
-    <t>Port Gamble Bay Wild</t>
-  </si>
-  <si>
     <t>Puyallup River Wild</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
     <t>Area 13B Miscellaneous Wild UnMarked</t>
   </si>
   <si>
-    <t>Area 7/7A Independent Wild UnMarked</t>
-  </si>
-  <si>
     <t>Willapa Bay Natural UnMarked</t>
   </si>
   <si>
@@ -244,9 +235,6 @@
     <t>Puyallup River Wild UnMarked</t>
   </si>
   <si>
-    <t>Port Gamble Bay Wild UnMarked</t>
-  </si>
-  <si>
     <t>Nooksack River Wild UnMarked</t>
   </si>
   <si>
@@ -256,9 +244,6 @@
     <t>Lake Washington Wild UnMarked</t>
   </si>
   <si>
-    <t>remove? Fixed input, not a real pop</t>
-  </si>
-  <si>
     <t xml:space="preserve">remove? Series is proxy "index" not an escapement estimate </t>
   </si>
   <si>
@@ -314,12 +299,6 @@
   </si>
   <si>
     <t>Baker (Skagit) Wild UnMarked</t>
-  </si>
-  <si>
-    <t>remove? does not match values in file "2006 through 2019 Drayton Harbor Streams COHO JK.xlsx" which are currently assigned to StockID-1 Nksk R Wild</t>
-  </si>
-  <si>
-    <t>unclear what this is</t>
   </si>
   <si>
     <t>both match mdb, neither match escp comp</t>
@@ -418,7 +397,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,12 +407,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,7 +450,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,25 +820,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -890,10 +862,10 @@
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -907,7 +879,7 @@
         <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>-122.465661</v>
@@ -940,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -954,7 +926,7 @@
         <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>-122.8242</v>
@@ -987,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1001,7 +973,7 @@
         <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>-122.45249200000001</v>
@@ -1034,10 +1006,10 @@
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="R4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1051,7 +1023,7 @@
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>-122.7836076</v>
@@ -1063,7 +1035,7 @@
         <v>95.4</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1090,7 +1062,7 @@
         <v>30</v>
       </c>
       <c r="Q5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1104,7 +1076,7 @@
         <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>-122.859826</v>
@@ -1116,7 +1088,7 @@
         <v>76.3</v>
       </c>
       <c r="H6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1143,7 +1115,7 @@
         <v>25</v>
       </c>
       <c r="Q6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1157,7 +1129,7 @@
         <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>-123.119288</v>
@@ -1190,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1204,7 +1176,7 @@
         <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>-123.01589439999999</v>
@@ -1216,7 +1188,7 @@
         <v>64.8</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1243,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="Q8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1257,7 +1229,7 @@
         <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>-122.702698</v>
@@ -1290,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1304,7 +1276,7 @@
         <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>-122.82063599999999</v>
@@ -1337,345 +1309,345 @@
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="3">
-        <v>-122.733811</v>
-      </c>
-      <c r="F11" s="3">
-        <v>48.972937000000002</v>
-      </c>
-      <c r="G11" s="3">
-        <v>115.1</v>
-      </c>
-      <c r="J11" s="3">
-        <v>1986</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11">
+        <v>-122.47416200000001</v>
+      </c>
+      <c r="F11">
+        <v>48.359836999999999</v>
+      </c>
+      <c r="G11">
+        <v>102.1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1986</v>
+      </c>
+      <c r="K11">
         <v>2017</v>
       </c>
-      <c r="L11" s="3">
-        <v>32</v>
-      </c>
-      <c r="M11" s="3">
-        <v>31</v>
-      </c>
-      <c r="N11" s="3">
-        <v>31</v>
-      </c>
-      <c r="O11" s="3">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>32</v>
+      </c>
+      <c r="M11">
+        <v>32</v>
+      </c>
+      <c r="N11">
+        <v>32</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>22</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12">
-        <v>-122.47416200000001</v>
-      </c>
-      <c r="F12">
-        <v>48.359836999999999</v>
-      </c>
-      <c r="G12">
-        <v>102.1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>1986</v>
-      </c>
-      <c r="K12">
-        <v>2017</v>
-      </c>
-      <c r="L12">
-        <v>32</v>
-      </c>
-      <c r="M12">
-        <v>32</v>
-      </c>
-      <c r="N12">
-        <v>32</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>22</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="C12" s="5">
+        <v>149</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-124.1692596</v>
+      </c>
+      <c r="F12" s="5">
+        <v>46.91656476</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2514.1999999999998</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1986</v>
+      </c>
+      <c r="K12" s="5">
+        <v>2018</v>
+      </c>
+      <c r="L12" s="5">
+        <v>33</v>
+      </c>
+      <c r="M12" s="5">
+        <v>32</v>
+      </c>
+      <c r="N12" s="5">
+        <v>32</v>
+      </c>
+      <c r="O12" s="5">
+        <v>32</v>
+      </c>
+      <c r="P12" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="6">
-        <v>149</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="6">
-        <v>-124.1692596</v>
-      </c>
-      <c r="F13" s="6">
-        <v>46.91656476</v>
-      </c>
-      <c r="G13" s="6">
-        <v>2514.1999999999998</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
-        <v>1986</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="C13">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13">
+        <v>-122.9091057</v>
+      </c>
+      <c r="F13">
+        <v>47.043614419999997</v>
+      </c>
+      <c r="G13">
+        <v>132.30000000000001</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1986</v>
+      </c>
+      <c r="K13">
         <v>2018</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13">
         <v>33</v>
       </c>
-      <c r="M13" s="6">
-        <v>32</v>
-      </c>
-      <c r="N13" s="6">
-        <v>32</v>
-      </c>
-      <c r="O13" s="6">
-        <v>32</v>
-      </c>
-      <c r="P13" s="6">
-        <v>30</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>32</v>
+      </c>
+      <c r="N13">
+        <v>32</v>
+      </c>
+      <c r="O13">
+        <v>33</v>
+      </c>
+      <c r="P13">
+        <v>18</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14">
-        <v>63</v>
-      </c>
-      <c r="D14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14">
-        <v>-122.9091057</v>
-      </c>
-      <c r="F14">
-        <v>47.043614419999997</v>
-      </c>
-      <c r="G14">
-        <v>132.30000000000001</v>
-      </c>
-      <c r="H14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>1986</v>
-      </c>
-      <c r="K14">
-        <v>2018</v>
-      </c>
-      <c r="L14">
-        <v>33</v>
-      </c>
-      <c r="M14">
-        <v>32</v>
-      </c>
-      <c r="N14">
-        <v>32</v>
-      </c>
-      <c r="O14">
-        <v>33</v>
-      </c>
-      <c r="P14">
-        <v>18</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="C14" s="3">
+        <v>107</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-123.129772</v>
+      </c>
+      <c r="F14" s="3">
+        <v>48.152718</v>
+      </c>
+      <c r="G14" s="3">
+        <v>129.69999999999999</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1986</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2017</v>
+      </c>
+      <c r="L14" s="3">
+        <v>32</v>
+      </c>
+      <c r="M14" s="3">
+        <v>32</v>
+      </c>
+      <c r="N14" s="3">
+        <v>32</v>
+      </c>
+      <c r="O14" s="2">
+        <v>13</v>
+      </c>
+      <c r="P14" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="4">
-        <v>107</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="4">
-        <v>-123.129772</v>
-      </c>
-      <c r="F15" s="4">
-        <v>48.152718</v>
-      </c>
-      <c r="G15" s="4">
-        <v>129.69999999999999</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="I15" s="4">
-        <v>1</v>
-      </c>
-      <c r="J15" s="4">
-        <v>1986</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="C15">
+        <v>115</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15">
+        <v>-123.0051816</v>
+      </c>
+      <c r="F15">
+        <v>48.023348120000001</v>
+      </c>
+      <c r="G15">
+        <v>301.3</v>
+      </c>
+      <c r="J15">
+        <v>1986</v>
+      </c>
+      <c r="K15">
         <v>2017</v>
       </c>
-      <c r="L15" s="4">
-        <v>32</v>
-      </c>
-      <c r="M15" s="4">
-        <v>32</v>
-      </c>
-      <c r="N15" s="4">
-        <v>32</v>
-      </c>
-      <c r="O15" s="2">
-        <v>13</v>
-      </c>
-      <c r="P15" s="4">
-        <v>10</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>32</v>
+      </c>
+      <c r="M15">
+        <v>32</v>
+      </c>
+      <c r="N15">
+        <v>32</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16">
-        <v>115</v>
-      </c>
-      <c r="D16" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16">
-        <v>-123.0051816</v>
-      </c>
-      <c r="F16">
-        <v>48.023348120000001</v>
-      </c>
-      <c r="G16">
-        <v>301.3</v>
-      </c>
-      <c r="J16">
-        <v>1986</v>
-      </c>
-      <c r="K16">
+      <c r="C16" s="4">
+        <v>111</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-123.56963399999999</v>
+      </c>
+      <c r="F16" s="4">
+        <v>48.148155000000003</v>
+      </c>
+      <c r="G16" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1986</v>
+      </c>
+      <c r="K16" s="4">
         <v>2017</v>
       </c>
-      <c r="L16">
-        <v>32</v>
-      </c>
-      <c r="M16">
-        <v>32</v>
-      </c>
-      <c r="N16">
-        <v>32</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>59</v>
+      <c r="L16" s="4">
+        <v>32</v>
+      </c>
+      <c r="M16" s="4">
+        <v>32</v>
+      </c>
+      <c r="N16" s="4">
+        <v>32</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="5">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E17" s="5">
-        <v>-123.56963399999999</v>
+        <v>-124.03316599999999</v>
       </c>
       <c r="F17" s="5">
-        <v>48.148155000000003</v>
+        <v>46.939467</v>
       </c>
       <c r="G17" s="5">
-        <v>13.7</v>
+        <v>211</v>
       </c>
       <c r="J17" s="5">
         <v>1986</v>
@@ -1687,10 +1659,10 @@
         <v>32</v>
       </c>
       <c r="M17" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N17" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O17" s="5">
         <v>0</v>
@@ -1699,419 +1671,419 @@
         <v>0</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6">
-        <v>157</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="6">
-        <v>-124.03316599999999</v>
-      </c>
-      <c r="F18" s="6">
-        <v>46.939467</v>
-      </c>
-      <c r="G18" s="6">
-        <v>211</v>
-      </c>
-      <c r="J18" s="6">
-        <v>1986</v>
-      </c>
-      <c r="K18" s="6">
+      <c r="C18" s="3">
+        <v>97</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-122.2145</v>
+      </c>
+      <c r="F18" s="3">
+        <v>47.351900000000001</v>
+      </c>
+      <c r="G18" s="3">
+        <v>339.3</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1986</v>
+      </c>
+      <c r="K18" s="3">
+        <v>2018</v>
+      </c>
+      <c r="L18" s="3">
+        <v>33</v>
+      </c>
+      <c r="M18" s="3">
+        <v>32</v>
+      </c>
+      <c r="N18" s="3">
+        <v>32</v>
+      </c>
+      <c r="O18" s="2">
+        <v>19</v>
+      </c>
+      <c r="P18" s="3">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19">
+        <v>-124.43052</v>
+      </c>
+      <c r="F19">
+        <v>47.749116000000001</v>
+      </c>
+      <c r="G19">
+        <v>263.10000000000002</v>
+      </c>
+      <c r="J19">
+        <v>1986</v>
+      </c>
+      <c r="K19">
         <v>2017</v>
       </c>
-      <c r="L18" s="6">
-        <v>32</v>
-      </c>
-      <c r="M18" s="6">
-        <v>30</v>
-      </c>
-      <c r="N18" s="6">
-        <v>30</v>
-      </c>
-      <c r="O18" s="6">
-        <v>0</v>
-      </c>
-      <c r="P18" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4">
-        <v>97</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="4">
-        <v>-122.2145</v>
-      </c>
-      <c r="F19" s="4">
-        <v>47.351900000000001</v>
-      </c>
-      <c r="G19" s="4">
-        <v>339.3</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I19" s="4">
-        <v>1</v>
-      </c>
-      <c r="J19" s="4">
-        <v>1986</v>
-      </c>
-      <c r="K19" s="4">
-        <v>2018</v>
-      </c>
-      <c r="L19" s="4">
-        <v>33</v>
-      </c>
-      <c r="M19" s="4">
-        <v>32</v>
-      </c>
-      <c r="N19" s="4">
-        <v>32</v>
-      </c>
-      <c r="O19" s="2">
-        <v>19</v>
-      </c>
-      <c r="P19" s="4">
-        <v>28</v>
-      </c>
-      <c r="Q19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>32</v>
+      </c>
+      <c r="M19">
+        <v>32</v>
+      </c>
+      <c r="N19">
+        <v>32</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C20">
-        <v>135</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20">
-        <v>-124.43052</v>
-      </c>
-      <c r="F20">
-        <v>47.749116000000001</v>
-      </c>
-      <c r="G20">
-        <v>263.10000000000002</v>
-      </c>
-      <c r="J20">
-        <v>1986</v>
-      </c>
-      <c r="K20">
+      <c r="C20" s="5">
+        <v>153</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="5">
+        <v>-124.054237</v>
+      </c>
+      <c r="F20" s="5">
+        <v>47.040880999999999</v>
+      </c>
+      <c r="G20" s="5">
+        <v>268.60000000000002</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1986</v>
+      </c>
+      <c r="K20" s="5">
         <v>2017</v>
       </c>
-      <c r="L20">
-        <v>32</v>
-      </c>
-      <c r="M20">
-        <v>32</v>
-      </c>
-      <c r="N20">
-        <v>32</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+      <c r="L20" s="5">
+        <v>32</v>
+      </c>
+      <c r="M20" s="5">
+        <v>32</v>
+      </c>
+      <c r="N20" s="5">
+        <v>32</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="6">
-        <v>153</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="6">
-        <v>-124.054237</v>
-      </c>
-      <c r="F21" s="6">
-        <v>47.040880999999999</v>
-      </c>
-      <c r="G21" s="6">
-        <v>268.60000000000002</v>
-      </c>
-      <c r="J21" s="6">
-        <v>1986</v>
-      </c>
-      <c r="K21" s="6">
+      <c r="C21" s="3">
+        <v>101</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-122.26042940000001</v>
+      </c>
+      <c r="F21" s="3">
+        <v>47.644992790000003</v>
+      </c>
+      <c r="G21" s="3">
+        <v>513.29999999999995</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1986</v>
+      </c>
+      <c r="K21" s="3">
         <v>2017</v>
       </c>
-      <c r="L21" s="6">
-        <v>32</v>
-      </c>
-      <c r="M21" s="6">
-        <v>32</v>
-      </c>
-      <c r="N21" s="6">
-        <v>32</v>
-      </c>
-      <c r="O21" s="6">
-        <v>0</v>
-      </c>
-      <c r="P21" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="L21" s="3">
+        <v>32</v>
+      </c>
+      <c r="M21" s="3">
+        <v>32</v>
+      </c>
+      <c r="N21" s="3">
+        <v>32</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="4">
-        <v>101</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="4">
-        <v>-122.26042940000001</v>
-      </c>
-      <c r="F22" s="4">
-        <v>47.644992790000003</v>
-      </c>
-      <c r="G22" s="4">
-        <v>513.29999999999995</v>
-      </c>
-      <c r="J22" s="4">
-        <v>1986</v>
-      </c>
-      <c r="K22" s="4">
-        <v>2017</v>
-      </c>
-      <c r="L22" s="4">
-        <v>32</v>
-      </c>
-      <c r="M22" s="4">
-        <v>32</v>
-      </c>
-      <c r="N22" s="4">
-        <v>32</v>
-      </c>
-      <c r="O22" s="4">
-        <v>0</v>
-      </c>
-      <c r="P22" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="R22" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22">
+        <v>-122.70121159999999</v>
+      </c>
+      <c r="F22">
+        <v>47.088108669999997</v>
+      </c>
+      <c r="G22">
+        <v>317.60000000000002</v>
+      </c>
+      <c r="H22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1986</v>
+      </c>
+      <c r="K22">
+        <v>2018</v>
+      </c>
+      <c r="L22">
+        <v>33</v>
+      </c>
+      <c r="M22">
+        <v>32</v>
+      </c>
+      <c r="N22">
+        <v>32</v>
+      </c>
+      <c r="O22">
+        <v>10</v>
+      </c>
+      <c r="P22">
+        <v>23</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="4">
+        <v>-122.597909</v>
+      </c>
+      <c r="F23" s="4">
+        <v>48.776489120000001</v>
+      </c>
+      <c r="G23" s="4">
+        <v>692.5</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1986</v>
+      </c>
+      <c r="K23" s="4">
+        <v>2018</v>
+      </c>
+      <c r="L23" s="4">
+        <v>33</v>
+      </c>
+      <c r="M23" s="4">
+        <v>32</v>
+      </c>
+      <c r="N23" s="4">
+        <v>32</v>
+      </c>
+      <c r="O23" s="2">
+        <v>14</v>
+      </c>
+      <c r="P23" s="4">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23">
-        <v>-122.70121159999999</v>
-      </c>
-      <c r="F23">
-        <v>47.088108669999997</v>
-      </c>
-      <c r="G23">
-        <v>317.60000000000002</v>
-      </c>
-      <c r="H23" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23">
+      <c r="E24">
+        <v>-122.4268386</v>
+      </c>
+      <c r="F24">
+        <v>47.268497920000001</v>
+      </c>
+      <c r="G24">
+        <v>580.1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24">
         <v>1</v>
       </c>
-      <c r="J23">
-        <v>1986</v>
-      </c>
-      <c r="K23">
+      <c r="J24">
+        <v>1986</v>
+      </c>
+      <c r="K24">
         <v>2018</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <v>33</v>
       </c>
-      <c r="M23">
-        <v>32</v>
-      </c>
-      <c r="N23">
-        <v>32</v>
-      </c>
-      <c r="O23">
-        <v>10</v>
-      </c>
-      <c r="P23">
-        <v>23</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="5">
-        <v>-122.597909</v>
-      </c>
-      <c r="F24" s="5">
-        <v>48.776489120000001</v>
-      </c>
-      <c r="G24" s="5">
-        <v>692.5</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="5">
-        <v>1</v>
-      </c>
-      <c r="J24" s="5">
-        <v>1986</v>
-      </c>
-      <c r="K24" s="5">
+      <c r="M24">
+        <v>32</v>
+      </c>
+      <c r="N24">
+        <v>32</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>30</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="5">
+        <v>139</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-124.3542841</v>
+      </c>
+      <c r="F25" s="5">
+        <v>47.53794224</v>
+      </c>
+      <c r="G25" s="5">
+        <v>381.2</v>
+      </c>
+      <c r="J25" s="5">
+        <v>1986</v>
+      </c>
+      <c r="K25" s="5">
         <v>2018</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L25" s="5">
         <v>33</v>
       </c>
-      <c r="M24" s="5">
-        <v>32</v>
-      </c>
-      <c r="N24" s="5">
-        <v>32</v>
-      </c>
-      <c r="O24" s="2">
-        <v>14</v>
-      </c>
-      <c r="P24" s="5">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="3">
-        <v>43</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="3">
-        <v>-122.57560700000001</v>
-      </c>
-      <c r="F25" s="3">
-        <v>47.833956000000001</v>
-      </c>
-      <c r="G25" s="3">
-        <v>12.8</v>
-      </c>
-      <c r="J25" s="3">
-        <v>1986</v>
-      </c>
-      <c r="K25" s="3">
-        <v>2017</v>
-      </c>
-      <c r="L25" s="3">
-        <v>26</v>
-      </c>
-      <c r="M25" s="3">
-        <v>25</v>
-      </c>
-      <c r="N25" s="3">
-        <v>25</v>
-      </c>
-      <c r="O25" s="3">
-        <v>0</v>
-      </c>
-      <c r="P25" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>77</v>
+      <c r="M25" s="5">
+        <v>32</v>
+      </c>
+      <c r="N25" s="5">
+        <v>32</v>
+      </c>
+      <c r="O25" s="5">
+        <v>33</v>
+      </c>
+      <c r="P25" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -2122,143 +2094,146 @@
         <v>33</v>
       </c>
       <c r="C26">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E26">
-        <v>-122.4268386</v>
+        <v>-124.64317</v>
       </c>
       <c r="F26">
-        <v>47.268497920000001</v>
+        <v>47.907395000000001</v>
       </c>
       <c r="G26">
-        <v>580.1</v>
-      </c>
-      <c r="H26" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
+        <v>761.6</v>
       </c>
       <c r="J26">
         <v>1986</v>
       </c>
       <c r="K26">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="L26">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M26">
         <v>32</v>
       </c>
       <c r="N26">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>127</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27">
+        <v>-124.64317</v>
+      </c>
+      <c r="F27">
+        <v>47.907395000000001</v>
+      </c>
+      <c r="G27">
+        <v>19.3</v>
+      </c>
+      <c r="J27">
+        <v>1986</v>
+      </c>
+      <c r="K27">
+        <v>2017</v>
+      </c>
+      <c r="L27">
+        <v>32</v>
+      </c>
+      <c r="M27">
+        <v>32</v>
+      </c>
+      <c r="N27">
         <v>30</v>
       </c>
-      <c r="Q26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="6">
-        <v>139</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="6">
-        <v>-124.3542841</v>
-      </c>
-      <c r="F27" s="6">
-        <v>47.53794224</v>
-      </c>
-      <c r="G27" s="6">
-        <v>381.2</v>
-      </c>
-      <c r="J27" s="6">
-        <v>1986</v>
-      </c>
-      <c r="K27" s="6">
-        <v>2018</v>
-      </c>
-      <c r="L27" s="6">
-        <v>33</v>
-      </c>
-      <c r="M27" s="6">
-        <v>32</v>
-      </c>
-      <c r="N27" s="6">
-        <v>32</v>
-      </c>
-      <c r="O27" s="6">
-        <v>33</v>
-      </c>
-      <c r="P27" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C28">
-        <v>131</v>
-      </c>
-      <c r="D28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28">
-        <v>-124.64317</v>
-      </c>
-      <c r="F28">
-        <v>47.907395000000001</v>
-      </c>
-      <c r="G28">
-        <v>761.6</v>
-      </c>
-      <c r="J28">
-        <v>1986</v>
-      </c>
-      <c r="K28">
+      <c r="C28" s="5">
+        <v>145</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-124.29792399999999</v>
+      </c>
+      <c r="F28" s="5">
+        <v>47.348188999999998</v>
+      </c>
+      <c r="G28" s="5">
+        <v>234.3</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1986</v>
+      </c>
+      <c r="K28" s="5">
         <v>2017</v>
       </c>
-      <c r="L28">
-        <v>32</v>
-      </c>
-      <c r="M28">
-        <v>32</v>
-      </c>
-      <c r="N28">
-        <v>30</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>57</v>
+      <c r="L28" s="5">
+        <v>32</v>
+      </c>
+      <c r="M28" s="5">
+        <v>32</v>
+      </c>
+      <c r="N28" s="5">
+        <v>32</v>
+      </c>
+      <c r="O28" s="5">
+        <v>0</v>
+      </c>
+      <c r="P28" s="5">
+        <v>29</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R28" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -2269,34 +2244,34 @@
         <v>36</v>
       </c>
       <c r="C29">
-        <v>127</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E29">
-        <v>-124.64317</v>
+        <v>-122.45678270000001</v>
       </c>
       <c r="F29">
-        <v>47.907395000000001</v>
+        <v>48.554918190000002</v>
       </c>
       <c r="G29">
-        <v>19.3</v>
+        <v>188.2</v>
       </c>
       <c r="J29">
         <v>1986</v>
       </c>
       <c r="K29">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="L29">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M29">
         <v>32</v>
       </c>
       <c r="N29">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O29">
         <v>0</v>
@@ -2305,63 +2280,60 @@
         <v>0</v>
       </c>
       <c r="Q29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="6">
-        <v>145</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="6">
-        <v>-124.29792399999999</v>
-      </c>
-      <c r="F30" s="6">
-        <v>47.348188999999998</v>
-      </c>
-      <c r="G30" s="6">
-        <v>234.3</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I30" s="6">
+      <c r="C30">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30">
+        <v>-122.3665</v>
+      </c>
+      <c r="F30">
+        <v>48.388056259999999</v>
+      </c>
+      <c r="G30">
+        <v>1050.5999999999999</v>
+      </c>
+      <c r="H30" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30">
         <v>1</v>
       </c>
-      <c r="J30" s="6">
-        <v>1986</v>
-      </c>
-      <c r="K30" s="6">
-        <v>2017</v>
-      </c>
-      <c r="L30" s="6">
-        <v>32</v>
-      </c>
-      <c r="M30" s="6">
-        <v>32</v>
-      </c>
-      <c r="N30" s="6">
-        <v>32</v>
-      </c>
-      <c r="O30" s="6">
-        <v>0</v>
-      </c>
-      <c r="P30" s="6">
+      <c r="J30">
+        <v>1986</v>
+      </c>
+      <c r="K30">
+        <v>2018</v>
+      </c>
+      <c r="L30">
+        <v>33</v>
+      </c>
+      <c r="M30">
+        <v>32</v>
+      </c>
+      <c r="N30">
+        <v>32</v>
+      </c>
+      <c r="O30">
         <v>29</v>
       </c>
-      <c r="Q30" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="R30" s="6" t="s">
-        <v>67</v>
+      <c r="P30">
+        <v>21</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2372,28 +2344,34 @@
         <v>38</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E31">
-        <v>-122.45678270000001</v>
+        <v>-123.11765699999999</v>
       </c>
       <c r="F31">
-        <v>48.554918190000002</v>
+        <v>47.339776000000001</v>
       </c>
       <c r="G31">
-        <v>188.2</v>
+        <v>106.1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>110</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
       </c>
       <c r="J31">
         <v>1986</v>
       </c>
       <c r="K31">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="L31">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M31">
         <v>32</v>
@@ -2405,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="P31">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="Q31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -2419,25 +2397,19 @@
         <v>39</v>
       </c>
       <c r="C32">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E32">
-        <v>-122.3665</v>
+        <v>-122.19891389999999</v>
       </c>
       <c r="F32">
-        <v>48.388056259999999</v>
+        <v>48.020066790000001</v>
       </c>
       <c r="G32">
-        <v>1050.5999999999999</v>
-      </c>
-      <c r="H32" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
+        <v>1358.8</v>
       </c>
       <c r="J32">
         <v>1986</v>
@@ -2455,13 +2427,13 @@
         <v>32</v>
       </c>
       <c r="O32">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="P32">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -2472,34 +2444,28 @@
         <v>40</v>
       </c>
       <c r="C33">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E33">
-        <v>-123.11765699999999</v>
+        <v>-122.39026749999999</v>
       </c>
       <c r="F33">
-        <v>47.339776000000001</v>
+        <v>48.243896329999998</v>
       </c>
       <c r="G33">
-        <v>106.1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
+        <v>694.2</v>
       </c>
       <c r="J33">
         <v>1986</v>
       </c>
       <c r="K33">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="L33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M33">
         <v>32</v>
@@ -2511,10 +2477,10 @@
         <v>0</v>
       </c>
       <c r="P33">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -2525,28 +2491,28 @@
         <v>41</v>
       </c>
       <c r="C34">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E34">
-        <v>-122.19891389999999</v>
+        <v>-123.7042368</v>
       </c>
       <c r="F34">
-        <v>48.020066790000001</v>
+        <v>48.155695020000003</v>
       </c>
       <c r="G34">
-        <v>1358.8</v>
+        <v>242.2</v>
       </c>
       <c r="J34">
         <v>1986</v>
       </c>
       <c r="K34">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="L34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M34">
         <v>32</v>
@@ -2555,13 +2521,13 @@
         <v>32</v>
       </c>
       <c r="O34">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P34">
         <v>0</v>
       </c>
       <c r="Q34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -2572,28 +2538,34 @@
         <v>42</v>
       </c>
       <c r="C35">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E35">
-        <v>-122.39026749999999</v>
+        <v>-124.09049</v>
       </c>
       <c r="F35">
-        <v>48.243896329999998</v>
+        <v>46.723579000000001</v>
       </c>
       <c r="G35">
-        <v>694.2</v>
+        <v>2028.2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>111</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
       </c>
       <c r="J35">
         <v>1986</v>
       </c>
       <c r="K35">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="L35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M35">
         <v>32</v>
@@ -2605,114 +2577,14 @@
         <v>0</v>
       </c>
       <c r="P35">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36">
-        <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36">
-        <v>-123.7042368</v>
-      </c>
-      <c r="F36">
-        <v>48.155695020000003</v>
-      </c>
-      <c r="G36">
-        <v>242.2</v>
-      </c>
-      <c r="J36">
-        <v>1986</v>
-      </c>
-      <c r="K36">
-        <v>2017</v>
-      </c>
-      <c r="L36">
-        <v>32</v>
-      </c>
-      <c r="M36">
-        <v>32</v>
-      </c>
-      <c r="N36">
-        <v>32</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37">
-        <v>161</v>
-      </c>
-      <c r="D37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37">
-        <v>-124.09049</v>
-      </c>
-      <c r="F37">
-        <v>46.723579000000001</v>
-      </c>
-      <c r="G37">
-        <v>2028.2</v>
-      </c>
-      <c r="H37" t="s">
-        <v>118</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <v>1986</v>
-      </c>
-      <c r="K37">
-        <v>2017</v>
-      </c>
-      <c r="L37">
-        <v>32</v>
-      </c>
-      <c r="M37">
-        <v>32</v>
-      </c>
-      <c r="N37">
-        <v>32</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>23</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R37" xr:uid="{AA8F3A9B-9786-4503-B548-981DD9035D8E}"/>
+  <autoFilter ref="A1:R35" xr:uid="{AA8F3A9B-9786-4503-B548-981DD9035D8E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>